<commit_message>
fix date to text
</commit_message>
<xml_diff>
--- a/templates/template_excel.xlsx
+++ b/templates/template_excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/damirs/PycharmProjects/WordGenerator/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leskhand\testProjects\WordGenerator\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43286966-CBF0-284B-9AAD-6A6ED1F1A13C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D50C77B-E12C-4F72-A04B-AE1324C3924F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="660" windowWidth="28480" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>г.Астана</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>филиал банка ЧСИ, где открыт счет</t>
+  </si>
+  <si>
+    <t>23.11.2025</t>
   </si>
 </sst>
 </file>
@@ -322,14 +325,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -614,102 +617,102 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="48.33203125" customWidth="1"/>
     <col min="5" max="5" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="30" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="52.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="52.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="141.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="141.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="20" customFormat="1" ht="112" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:26" s="19" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="O1" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="P1" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="Q1" s="20" t="s">
+      <c r="Q1" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="20" t="s">
+      <c r="R1" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="S1" s="20" t="s">
+      <c r="S1" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="T1" s="20" t="s">
+      <c r="T1" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="U1" s="20" t="s">
+      <c r="U1" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="V1" s="20" t="s">
+      <c r="V1" s="19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -777,7 +780,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="str">
         <f ca="1">TEXT(TODAY(),"ДД.ММ.ГГГГ")</f>
         <v>25.12.2025</v>
@@ -797,8 +800,8 @@
       <c r="F3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="19">
-        <v>45984</v>
+      <c r="G3" s="21" t="s">
+        <v>51</v>
       </c>
       <c r="H3" s="14" t="s">
         <v>4</v>
@@ -857,7 +860,7 @@
       <c r="Y3" s="7"/>
       <c r="Z3" s="7"/>
     </row>
-    <row r="4" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -884,7 +887,7 @@
       <c r="Y4" s="7"/>
       <c r="Z4" s="7"/>
     </row>
-    <row r="5" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -912,7 +915,7 @@
       <c r="Y5" s="7"/>
       <c r="Z5" s="7"/>
     </row>
-    <row r="6" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -940,7 +943,7 @@
       <c r="Y6" s="7"/>
       <c r="Z6" s="7"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -968,7 +971,7 @@
       <c r="Y7" s="7"/>
       <c r="Z7" s="7"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -996,7 +999,7 @@
       <c r="Y8" s="7"/>
       <c r="Z8" s="7"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -1024,7 +1027,7 @@
       <c r="Y9" s="7"/>
       <c r="Z9" s="7"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -1052,7 +1055,7 @@
       <c r="Y10" s="7"/>
       <c r="Z10" s="7"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1080,7 +1083,7 @@
       <c r="Y11" s="7"/>
       <c r="Z11" s="7"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1108,7 +1111,7 @@
       <c r="Y12" s="7"/>
       <c r="Z12" s="7"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1136,7 +1139,7 @@
       <c r="Y13" s="7"/>
       <c r="Z13" s="7"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1164,7 +1167,7 @@
       <c r="Y14" s="7"/>
       <c r="Z14" s="7"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -1192,7 +1195,7 @@
       <c r="Y15" s="7"/>
       <c r="Z15" s="7"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1220,7 +1223,7 @@
       <c r="Y16" s="7"/>
       <c r="Z16" s="7"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -1248,7 +1251,7 @@
       <c r="Y17" s="7"/>
       <c r="Z17" s="7"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -1276,7 +1279,7 @@
       <c r="Y18" s="7"/>
       <c r="Z18" s="7"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1304,7 +1307,7 @@
       <c r="Y19" s="7"/>
       <c r="Z19" s="7"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -1332,7 +1335,7 @@
       <c r="Y20" s="7"/>
       <c r="Z20" s="7"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -1360,7 +1363,7 @@
       <c r="Y21" s="7"/>
       <c r="Z21" s="7"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -1388,7 +1391,7 @@
       <c r="Y22" s="7"/>
       <c r="Z22" s="7"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -1416,7 +1419,7 @@
       <c r="Y23" s="7"/>
       <c r="Z23" s="7"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -1444,7 +1447,7 @@
       <c r="Y24" s="7"/>
       <c r="Z24" s="7"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -1472,7 +1475,7 @@
       <c r="Y25" s="7"/>
       <c r="Z25" s="7"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -1500,7 +1503,7 @@
       <c r="Y26" s="7"/>
       <c r="Z26" s="7"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -1528,7 +1531,7 @@
       <c r="Y27" s="7"/>
       <c r="Z27" s="7"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>

</xml_diff>